<commit_message>
mptt working well for taxa, have removed dates from metadata and added to datasets, about to branch off to test handson
</commit_message>
<xml_diff>
--- a/core/static/fatality_data_for_upload.xlsx
+++ b/core/static/fatality_data_for_upload.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4301">
   <si>
     <t>name</t>
   </si>
@@ -9506,6 +9506,9 @@
     <t>Poecilodryas superciliosa</t>
   </si>
   <si>
+    <t>Pogoniulus atroflavus</t>
+  </si>
+  <si>
     <t>Pogoniulus bilineatus</t>
   </si>
   <si>
@@ -12429,21 +12432,6 @@
   </si>
   <si>
     <t>Turdus olivaceus transvaalensis</t>
-  </si>
-  <si>
-    <t>Turdus philomelos</t>
-  </si>
-  <si>
-    <t>Turdus philomelos clarkei</t>
-  </si>
-  <si>
-    <t>Turdus philomelos hebridensis</t>
-  </si>
-  <si>
-    <t>Turdus philomelos nataliae</t>
-  </si>
-  <si>
-    <t>Turdus philomelos philomelos</t>
   </si>
   <si>
     <t>Turdus smithi</t>
@@ -29313,7 +29301,7 @@
   <sheetProtection autoFilter="1" deleteColumns="1" deleteRows="1" formatCells="1" formatColumns="1" formatRows="1" insertColumns="1" insertHyperlinks="1" insertRows="1" objects="0" pivotTables="1" scenarios="0" selectLockedCells="0" selectUnlockedCells="0" sheet="1" sort="1"/>
   <dataValidations count="4">
     <dataValidation allowBlank="0" error="Invalid genus. Please see the &quot;Valid Species&quot; sheet to view allowed species." prompt="Please see the &quot;Valid Species&quot; sheet to view allowed species." promptTitle="Restricted list" showErrorMessage="1" showInputMessage="1" sqref="A2:A1048576" type="list">
-      <formula1>='Valid Species'!A1:A4302</formula1>
+      <formula1>='Valid Species'!A1:A4298</formula1>
     </dataValidation>
     <dataValidation allowBlank="0" error="Invalid. Please enter a negative number between -21 and -35." operator="between" prompt="Please enter a negative number between -21 and -35." showErrorMessage="1" showInputMessage="1" sqref="B1:B2000" type="decimal">
       <formula1>-35</formula1>
@@ -29337,7 +29325,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4302"/>
+  <dimension ref="A1:A4298"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -47962,7 +47950,7 @@
     </row>
     <row r="3724" spans="1:1">
       <c r="A3724" t="s">
-        <v>3726</v>
+        <v>3727</v>
       </c>
     </row>
     <row r="3725" spans="1:1">
@@ -50833,26 +50821,6 @@
     <row r="4298" spans="1:1">
       <c r="A4298" t="s">
         <v>4300</v>
-      </c>
-    </row>
-    <row r="4299" spans="1:1">
-      <c r="A4299" t="s">
-        <v>4301</v>
-      </c>
-    </row>
-    <row r="4300" spans="1:1">
-      <c r="A4300" t="s">
-        <v>4302</v>
-      </c>
-    </row>
-    <row r="4301" spans="1:1">
-      <c r="A4301" t="s">
-        <v>4303</v>
-      </c>
-    </row>
-    <row r="4302" spans="1:1">
-      <c r="A4302" t="s">
-        <v>4304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>